<commit_message>
Added documentation, deleted more test files
</commit_message>
<xml_diff>
--- a/Table of expected vs. calculated dimensions.xlsx
+++ b/Table of expected vs. calculated dimensions.xlsx
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -539,11 +539,11 @@
         <v>1.3264</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D27" si="0">C5-B5</f>
+        <f t="shared" ref="D5" si="0">C5-B5</f>
         <v>-0.13850000000000007</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E31" si="1">D5/B5 * 100</f>
+        <f t="shared" ref="E5" si="1">D5/B5 * 100</f>
         <v>-9.4545702778346694</v>
       </c>
       <c r="F5">
@@ -562,11 +562,11 @@
         <v>1.45964</v>
       </c>
       <c r="D6">
-        <f>C6-B6</f>
+        <f t="shared" ref="D6:D12" si="3">C6-B6</f>
         <v>-0.17825999999999986</v>
       </c>
       <c r="E6">
-        <f>D6/B6 * 100</f>
+        <f t="shared" ref="E6:E12" si="4">D6/B6 * 100</f>
         <v>-10.883448317968123</v>
       </c>
       <c r="F6">
@@ -585,11 +585,11 @@
         <v>1.72811</v>
       </c>
       <c r="D7">
-        <f>C7-B7</f>
+        <f t="shared" si="3"/>
         <v>-0.27188999999999997</v>
       </c>
       <c r="E7">
-        <f>D7/B7 * 100</f>
+        <f t="shared" si="4"/>
         <v>-13.594499999999998</v>
       </c>
       <c r="F7">
@@ -608,11 +608,11 @@
         <v>1.2056</v>
       </c>
       <c r="D8">
-        <f>C8-B8</f>
+        <f t="shared" si="3"/>
         <v>7.6449999999999907E-2</v>
       </c>
       <c r="E8">
-        <f>D8/B8 * 100</f>
+        <f t="shared" si="4"/>
         <v>6.7705796395518654</v>
       </c>
       <c r="F8">
@@ -631,11 +631,11 @@
         <v>1.4940800000000001</v>
       </c>
       <c r="D9">
-        <f>C9-B9</f>
+        <f t="shared" si="3"/>
         <v>-0.50591999999999993</v>
       </c>
       <c r="E9">
-        <f>D9/B9 * 100</f>
+        <f t="shared" si="4"/>
         <v>-25.295999999999996</v>
       </c>
       <c r="F9">
@@ -654,11 +654,11 @@
         <v>1.1967699999999999</v>
       </c>
       <c r="D10">
-        <f>C10-B10</f>
+        <f t="shared" si="3"/>
         <v>0.11556999999999995</v>
       </c>
       <c r="E10">
-        <f>D10/B10 * 100</f>
+        <f t="shared" si="4"/>
         <v>10.689049204587493</v>
       </c>
       <c r="F10">
@@ -677,11 +677,11 @@
         <v>1.5656000000000001</v>
       </c>
       <c r="D11">
-        <f>C11-B11</f>
+        <f t="shared" si="3"/>
         <v>-0.36839999999999984</v>
       </c>
       <c r="E11">
-        <f>D11/B11 * 100</f>
+        <f t="shared" si="4"/>
         <v>-19.048603929679413</v>
       </c>
       <c r="F11">
@@ -700,11 +700,11 @@
         <v>1.7458800000000001</v>
       </c>
       <c r="D12">
-        <f>C12-B12</f>
+        <f t="shared" si="3"/>
         <v>-0.2541199999999999</v>
       </c>
       <c r="E12">
-        <f>D12/B12 * 100</f>
+        <f t="shared" si="4"/>
         <v>-12.705999999999996</v>
       </c>
       <c r="F12">

</xml_diff>

<commit_message>
Added more tester files and added more checks to the code
</commit_message>
<xml_diff>
--- a/Table of expected vs. calculated dimensions.xlsx
+++ b/Table of expected vs. calculated dimensions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A3:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>